<commit_message>
final tried, accuracy 0
</commit_message>
<xml_diff>
--- a/project final/data/코드북_features.xlsx
+++ b/project final/data/코드북_features.xlsx
@@ -1,37 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siheon/pi-heaan/project progress/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siheon/pi-heaan/project final/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:4000b_{076D6B73-B86D-3D42-B4A2-979EA1A6F122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EBA41A-F127-DE4E-B8FD-19FB31D7EC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22540" yWindow="-3100" windowWidth="22540" windowHeight="21100" tabRatio="774"/>
+    <workbookView xWindow="28800" yWindow="-1980" windowWidth="27320" windowHeight="19980" tabRatio="774" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="코드북" sheetId="30" r:id="rId1"/>
+    <sheet name="코드북 new" sheetId="31" r:id="rId1"/>
+    <sheet name="코드북" sheetId="30" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="359">
   <si>
     <t>성별</t>
   </si>
@@ -1322,8 +1312,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="32">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1568,6 +1558,13 @@
       <b/>
       <sz val="14"/>
       <color theme="4"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -2054,7 +2051,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2067,7 +2064,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2091,34 +2088,25 @@
     <xf numFmtId="14" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2165,16 +2153,16 @@
     <cellStyle name="좋음" xfId="41" builtinId="26" customBuiltin="1"/>
     <cellStyle name="출력" xfId="42" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 10 2 10" xfId="43"/>
-    <cellStyle name="표준 2" xfId="44"/>
-    <cellStyle name="표준 2 11 10" xfId="45"/>
-    <cellStyle name="표준 2 2" xfId="46"/>
-    <cellStyle name="표준 2 3" xfId="47"/>
-    <cellStyle name="표준 2 4" xfId="48"/>
-    <cellStyle name="표준 2 5" xfId="49"/>
-    <cellStyle name="표준 3" xfId="50"/>
-    <cellStyle name="표준 7" xfId="51"/>
-    <cellStyle name="headerStyle" xfId="19"/>
+    <cellStyle name="표준 10 2 10" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="표준 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="표준 2 11 10" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="표준 2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="표준 2 3" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="표준 2 4" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="표준 2 5" xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="표준 3" xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="표준 7" xfId="51" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="headerStyle" xfId="19" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2475,11 +2463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D946C9-8416-3C43-9E63-CCD817186C07}">
   <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:IV2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2527,6 +2515,1683 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3" spans="1:7" hidden="1">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" hidden="1">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" hidden="1">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" hidden="1">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="18">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" hidden="1">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" hidden="1">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" hidden="1">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" hidden="1">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" hidden="1">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" hidden="1">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="2">
+        <v>45</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="2">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1">
+      <c r="A50" s="2">
+        <v>48</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1">
+      <c r="A51" s="2">
+        <v>49</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1">
+      <c r="A59" s="2">
+        <v>57</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1">
+      <c r="A60" s="2">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1">
+      <c r="A61" s="2">
+        <v>59</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1">
+      <c r="A62" s="2">
+        <v>60</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1">
+      <c r="A63" s="2">
+        <v>61</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1">
+      <c r="A64" s="2">
+        <v>62</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1">
+      <c r="A65" s="2">
+        <v>63</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1">
+      <c r="A66" s="2">
+        <v>64</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1">
+      <c r="A67" s="2">
+        <v>65</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" hidden="1">
+      <c r="A69" s="2">
+        <v>67</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1">
+      <c r="A70" s="2">
+        <v>68</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" hidden="1">
+      <c r="A71" s="2">
+        <v>69</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" hidden="1">
+      <c r="A72" s="2">
+        <v>70</v>
+      </c>
+      <c r="C72" t="s">
+        <v>353</v>
+      </c>
+      <c r="D72" t="s">
+        <v>354</v>
+      </c>
+      <c r="E72" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" hidden="1">
+      <c r="A73" s="2">
+        <v>71</v>
+      </c>
+      <c r="C73" t="s">
+        <v>356</v>
+      </c>
+      <c r="D73" t="s">
+        <v>357</v>
+      </c>
+      <c r="E73" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1">
+      <c r="A74" s="2">
+        <v>72</v>
+      </c>
+      <c r="C74" t="s">
+        <v>347</v>
+      </c>
+      <c r="D74" t="s">
+        <v>348</v>
+      </c>
+      <c r="E74" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1">
+      <c r="A75" s="2">
+        <v>73</v>
+      </c>
+      <c r="C75" t="s">
+        <v>350</v>
+      </c>
+      <c r="D75" t="s">
+        <v>351</v>
+      </c>
+      <c r="E75" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="32" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.6640625" customWidth="1"/>
+    <col min="8" max="256" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20">
+      <c r="A1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>1</v>
@@ -2534,7 +4199,7 @@
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2553,13 +4218,13 @@
       <c r="B4" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="15" t="s">
         <v>273</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2574,7 +4239,7 @@
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -2595,7 +4260,7 @@
       <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -2616,7 +4281,7 @@
       <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -2637,7 +4302,7 @@
       <c r="B8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -2658,7 +4323,7 @@
       <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="12" t="s">
         <v>280</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -2679,7 +4344,7 @@
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="12" t="s">
         <v>281</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -2700,7 +4365,7 @@
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="12" t="s">
         <v>218</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -2719,7 +4384,7 @@
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -2740,7 +4405,7 @@
       <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -2761,7 +4426,7 @@
       <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -2782,13 +4447,13 @@
       <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="4" t="s">
         <v>210</v>
       </c>
       <c r="F15" s="10" t="s">
@@ -2805,13 +4470,13 @@
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="4" t="s">
         <v>211</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -2828,13 +4493,13 @@
       <c r="B17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="4" t="s">
         <v>212</v>
       </c>
       <c r="F17" s="10" t="s">
@@ -2851,13 +4516,13 @@
       <c r="B18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="4" t="s">
         <v>213</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -2874,13 +4539,13 @@
       <c r="B19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="4" t="s">
         <v>214</v>
       </c>
       <c r="F19" s="10" t="s">
@@ -2897,13 +4562,13 @@
       <c r="B20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="4" t="s">
         <v>215</v>
       </c>
       <c r="F20" s="10" t="s">
@@ -2920,13 +4585,13 @@
       <c r="B21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="4" t="s">
         <v>216</v>
       </c>
       <c r="F21" s="10" t="s">
@@ -2943,13 +4608,13 @@
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="4" t="s">
         <v>217</v>
       </c>
       <c r="F22" s="10" t="s">
@@ -2966,7 +4631,7 @@
       <c r="B23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2989,7 +4654,7 @@
       <c r="B24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="12" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -3012,7 +4677,7 @@
       <c r="B25" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="12" t="s">
         <v>69</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -3035,7 +4700,7 @@
       <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D26" s="6" t="s">
@@ -3058,7 +4723,7 @@
       <c r="B27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -3081,7 +4746,7 @@
       <c r="B28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -3104,7 +4769,7 @@
       <c r="B29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="12" t="s">
         <v>235</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -3127,7 +4792,7 @@
       <c r="B30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -3150,7 +4815,7 @@
       <c r="B31" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -3173,7 +4838,7 @@
       <c r="B32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -3196,7 +4861,7 @@
       <c r="B33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="12" t="s">
         <v>88</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -3219,7 +4884,7 @@
       <c r="B34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -3242,7 +4907,7 @@
       <c r="B35" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="12" t="s">
         <v>93</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -3265,7 +4930,7 @@
       <c r="B36" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="12" t="s">
         <v>97</v>
       </c>
       <c r="D36" s="6" t="s">
@@ -3288,7 +4953,7 @@
       <c r="B37" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -3311,19 +4976,19 @@
       <c r="B38" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="G38" s="10" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3334,19 +4999,19 @@
       <c r="B39" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="G39" s="10" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3357,7 +5022,7 @@
       <c r="B40" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -3380,7 +5045,7 @@
       <c r="B41" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -3403,7 +5068,7 @@
       <c r="B42" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="12" t="s">
         <v>116</v>
       </c>
       <c r="D42" s="6" t="s">
@@ -3426,7 +5091,7 @@
       <c r="B43" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -3449,7 +5114,7 @@
       <c r="B44" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D44" s="6" t="s">
@@ -3472,7 +5137,7 @@
       <c r="B45" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="12" t="s">
         <v>241</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -3495,7 +5160,7 @@
       <c r="B46" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D46" s="6" t="s">
@@ -3518,7 +5183,7 @@
       <c r="B47" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="12" t="s">
         <v>129</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -3541,13 +5206,13 @@
       <c r="B48" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="6" t="s">
         <v>251</v>
       </c>
       <c r="F48" s="5" t="s">
@@ -3564,13 +5229,13 @@
       <c r="B49" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C49" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E49" s="6" t="s">
         <v>254</v>
       </c>
       <c r="F49" s="7" t="s">
@@ -3587,13 +5252,13 @@
       <c r="B50" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="6" t="s">
         <v>255</v>
       </c>
       <c r="F50" s="7" t="s">
@@ -3610,7 +5275,7 @@
       <c r="B51" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="12" t="s">
         <v>139</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -3633,7 +5298,7 @@
       <c r="B52" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="12" t="s">
         <v>142</v>
       </c>
       <c r="D52" s="6" t="s">
@@ -3656,7 +5321,7 @@
       <c r="B53" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="12" t="s">
         <v>145</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -3679,7 +5344,7 @@
       <c r="B54" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="6" t="s">
@@ -3702,7 +5367,7 @@
       <c r="B55" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -3725,7 +5390,7 @@
       <c r="B56" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="12" t="s">
         <v>151</v>
       </c>
       <c r="D56" s="6" t="s">
@@ -3748,7 +5413,7 @@
       <c r="B57" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="12" t="s">
         <v>158</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -3771,7 +5436,7 @@
       <c r="B58" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="12" t="s">
         <v>161</v>
       </c>
       <c r="D58" s="6" t="s">
@@ -3794,7 +5459,7 @@
       <c r="B59" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C59" s="12" t="s">
         <v>163</v>
       </c>
       <c r="D59" s="6" t="s">
@@ -3817,7 +5482,7 @@
       <c r="B60" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="12" t="s">
         <v>165</v>
       </c>
       <c r="D60" s="6" t="s">
@@ -3840,7 +5505,7 @@
       <c r="B61" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="12" t="s">
         <v>166</v>
       </c>
       <c r="D61" s="6" t="s">
@@ -3863,7 +5528,7 @@
       <c r="B62" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="C62" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D62" s="6" t="s">
@@ -3886,7 +5551,7 @@
       <c r="B63" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C63" s="12" t="s">
         <v>169</v>
       </c>
       <c r="D63" s="6" t="s">
@@ -3909,7 +5574,7 @@
       <c r="B64" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C64" s="12" t="s">
         <v>172</v>
       </c>
       <c r="D64" s="6" t="s">
@@ -3932,7 +5597,7 @@
       <c r="B65" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C65" s="12" t="s">
         <v>175</v>
       </c>
       <c r="D65" s="6" t="s">
@@ -3955,13 +5620,13 @@
       <c r="B66" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C66" s="18" t="s">
+      <c r="C66" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="4" t="s">
         <v>246</v>
       </c>
       <c r="F66" s="10" t="s">
@@ -3978,16 +5643,16 @@
       <c r="B67" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C67" s="18" t="s">
+      <c r="C67" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D67" s="15" t="s">
+      <c r="D67" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="E67" s="15" t="s">
+      <c r="E67" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="F67" s="15" t="s">
+      <c r="F67" s="4" t="s">
         <v>185</v>
       </c>
       <c r="G67" s="5" t="s">
@@ -4001,16 +5666,16 @@
       <c r="B68" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C68" s="18" t="s">
+      <c r="C68" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="D68" s="15" t="s">
+      <c r="D68" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="E68" s="15" t="s">
+      <c r="E68" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="F68" s="15" t="s">
+      <c r="F68" s="4" t="s">
         <v>188</v>
       </c>
       <c r="G68" s="5" t="s">
@@ -4024,16 +5689,16 @@
       <c r="B69" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D69" s="15" t="s">
+      <c r="D69" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="E69" s="15" t="s">
+      <c r="E69" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="F69" s="15" t="s">
+      <c r="F69" s="4" t="s">
         <v>191</v>
       </c>
       <c r="G69" s="5" t="s">
@@ -4047,16 +5712,16 @@
       <c r="B70" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C70" s="18" t="s">
+      <c r="C70" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="E70" s="15" t="s">
+      <c r="E70" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="F70" s="15" t="s">
+      <c r="F70" s="4" t="s">
         <v>194</v>
       </c>
       <c r="G70" s="5" t="s">
@@ -4070,16 +5735,16 @@
       <c r="B71" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C71" s="18" t="s">
+      <c r="C71" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="D71" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="E71" s="15" t="s">
+      <c r="E71" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="F71" s="15" t="s">
+      <c r="F71" s="4" t="s">
         <v>197</v>
       </c>
       <c r="G71" s="5" t="s">

</xml_diff>